<commit_message>
After much trial and error, got the maven plugin unit tests to work both standalone (using Maven) and within Eclipse.
Intermediate checkin of some of the dependency code (not fully
implemented).
</commit_message>
<xml_diff>
--- a/SPDX-fields-maven-mapping.xlsx
+++ b/SPDX-fields-maven-mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="137">
   <si>
     <t>2 SPDX Document Information</t>
   </si>
@@ -224,9 +224,6 @@
     <t>"CC0-1.0" (SPDX standard licenase creative commons version 1.0)</t>
   </si>
   <si>
-    <t>RDF Document URI</t>
-  </si>
-  <si>
     <t>plugin property parameter spdxDocumentUrl - default value "http://spdx.org/spdxpackages/${project.name}-${project.version}"</t>
   </si>
   <si>
@@ -1361,6 +1358,27 @@
       </rPr>
       <t xml:space="preserve"> Annotation Comment</t>
     </r>
+  </si>
+  <si>
+    <t>Generated</t>
+  </si>
+  <si>
+    <t>documentAnnotation and packageAnnotation for document and package annotations resp.</t>
+  </si>
+  <si>
+    <t>annotator</t>
+  </si>
+  <si>
+    <t>annotationDate</t>
+  </si>
+  <si>
+    <t>annotationType</t>
+  </si>
+  <si>
+    <t>annotationComment</t>
+  </si>
+  <si>
+    <t>documentAnnotations and packageAnnotations for document and package annotations resp.</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1421,12 +1439,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1443,7 +1455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1458,13 +1470,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1804,13 +1809,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1824,7 +1829,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -1833,7 +1838,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1852,7 +1857,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
@@ -1869,165 +1874,177 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="C5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="47.25">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="31.5">
       <c r="A9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5">
+      <c r="A10" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5">
+      <c r="A15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.5">
-      <c r="A10" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" ht="47.25">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="8" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="78.75">
+      <c r="A18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="31.5">
-      <c r="A16" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="78.75">
-      <c r="A19" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="63">
+      <c r="A19" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="63">
-      <c r="A20" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2037,8 +2054,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:4" ht="31.5">
+      <c r="A21" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2049,442 +2066,455 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="31.5">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="31.5">
-      <c r="A23" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="31.5">
+      <c r="A26" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="31.5">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="6" t="s">
         <v>98</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31.5">
-      <c r="A28" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="63">
+      <c r="A28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="63">
-      <c r="A29" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="31.5">
+      <c r="A30" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="31.5">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="31.5">
-      <c r="A32" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" ht="31.5">
+      <c r="A37" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" ht="31.5">
-      <c r="A38" s="9" t="s">
+      <c r="D37" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="9" t="s">
+    <row r="39" spans="1:4" ht="47.25">
+      <c r="A39" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="D39" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="47.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="4" t="s">
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="47.25">
-      <c r="A41" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="D41" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="31.5">
+      <c r="A42" s="6" t="s">
         <v>113</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="31.5">
-      <c r="A43" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="9" t="s">
-        <v>116</v>
+      <c r="A46" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="31.5">
+      <c r="A50" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>8</v>
+      <c r="C50" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="31.5">
-      <c r="A51" s="9" t="s">
-        <v>121</v>
+      <c r="A51" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="31.5">
       <c r="A52" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="31.5">
       <c r="A53" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="31.5">
       <c r="A54" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="31.5">
-      <c r="A55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="6" t="s">
         <v>122</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="9" t="s">
+    <row r="58" spans="1:4" ht="31.5">
+      <c r="A58" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" t="s">
+        <v>133</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="C61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="C62" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="C63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="3" t="s">
-        <v>9</v>
+      <c r="A66" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding snippets.  Also fixed bugs with file specific information.  Stable support for new 2.1 features
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/SPDX-fields-maven-mapping.xlsx
+++ b/SPDX-fields-maven-mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="159">
   <si>
     <t>2 SPDX Document Information</t>
   </si>
@@ -1417,6 +1417,39 @@
   </si>
   <si>
     <t>plugin paramater externalReferences</t>
+  </si>
+  <si>
+    <t>N/A - generated</t>
+  </si>
+  <si>
+    <t>Identifier of the file which includes the snippet (the file is identified through the patch specific file info)</t>
+  </si>
+  <si>
+    <t>Snippets are plugin paramaters in the PathSpecificFileInformtion paramater - to use, specify a path specific file info for a file containing the snippet.  Include all of the correct (and defualt) copyright info (it will not take it from the default file info if not provided).  Add a sub-paramater snippets which is a list of SnippetInfo.</t>
+  </si>
+  <si>
+    <t>byteRange SnippetInfo parameter - String formated same as the tag/value format</t>
+  </si>
+  <si>
+    <t>lineRange SnippetInfo parameter - String formated same as the tag/value format</t>
+  </si>
+  <si>
+    <t>concludedLicense SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>licenseInfoInSnippet SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>licenseComment SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>copyrightText SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>comment SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>name SnippetInfo parameter</t>
   </si>
 </sst>
 </file>
@@ -1516,13 +1549,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1532,6 +1559,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1866,10 +1897,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A46" sqref="A46:XFD48"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2120,10 +2151,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="31.5">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
         <v>105</v>
       </c>
@@ -2260,22 +2291,22 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
@@ -2399,82 +2430,104 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:4" ht="110.25">
+      <c r="A49" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="5"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="11" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="8" t="s">
+      <c r="B50" s="13"/>
+      <c r="C50" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="31.5">
+      <c r="A51" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="8" t="s">
+      <c r="B51" s="13"/>
+      <c r="C51" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="31.5">
+      <c r="A52" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="8" t="s">
+      <c r="B52" s="13"/>
+      <c r="C52" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="31.5">
+      <c r="A53" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="5"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="11" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="11" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="5"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="11" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="5"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="5"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="11" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="5"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="11" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="5"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="11" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
@@ -2616,7 +2669,7 @@
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C74" t="s">

</xml_diff>

<commit_message>
Fix relative file paths for directory specific information.  Final changes for SPDX 2.1 bake-off
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/SPDX-fields-maven-mapping.xlsx
+++ b/SPDX-fields-maven-mapping.xlsx
@@ -1897,10 +1897,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Update copyrights in preparation for the move to the SPDX git repo.  Note that the project has not been accepted by Apache, so the copyrights labels need to be modified.  The license list has also been updated to the latest version.
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/SPDX-fields-maven-mapping.xlsx
+++ b/SPDX-fields-maven-mapping.xlsx
@@ -1897,10 +1897,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Fix incorrect field name for spdxDocumentNamespace
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/SPDX-fields-maven-mapping.xlsx
+++ b/SPDX-fields-maven-mapping.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\spdx-maven-plugin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A56A517-B9CF-44AC-8D29-B05898C37883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1125" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="72" yWindow="732" windowWidth="22968" windowHeight="11628" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,9 +105,6 @@
     <t>"CC0-1.0" (SPDX standard licenase creative commons version 1.0)</t>
   </si>
   <si>
-    <t>plugin property parameter spdxDocumentUrl - default value "http://spdx.org/spdxpackages/${project.name}-${project.version}"</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -1450,12 +1453,15 @@
   </si>
   <si>
     <t>name SnippetInfo parameter</t>
+  </si>
+  <si>
+    <t>plugin property parameter spdxDocumentNamespace - default value "http://spdx.org/spdxpackages/${project.name}-${project.version}"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -1569,6 +1575,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1893,28 +1907,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="3" max="3" width="45.3984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.8984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>8</v>
@@ -1923,7 +1937,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1942,13 +1956,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5">
+    <row r="4" spans="1:5" ht="31.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1959,135 +1973,135 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="31.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.2">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="62.4">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="31.5">
+    <row r="9" spans="1:5" ht="31.2">
       <c r="A9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.2">
+      <c r="A10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.5">
-      <c r="A10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5">
+    <row r="15" spans="1:5" ht="31.2">
       <c r="A15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -2097,220 +2111,220 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="93.6">
+      <c r="A18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="78.75">
-      <c r="A18" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="62.4">
+      <c r="A19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="63">
-      <c r="A19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="31.2">
+      <c r="A21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="31.5">
-      <c r="A21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="D21" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="31.2">
+      <c r="A22" s="10" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="31.5">
-      <c r="A22" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="31.2">
+      <c r="A23" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="31.5">
-      <c r="A23" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="C23" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="31.2">
+      <c r="A27" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="31.5">
-      <c r="A27" s="6" t="s">
+      <c r="D27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="31.2">
+      <c r="A28" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31.5">
-      <c r="A28" s="6" t="s">
+      <c r="D28" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="62.4">
+      <c r="A29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="63">
-      <c r="A29" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="31.2">
+      <c r="A31" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="31.5">
-      <c r="A31" s="6" t="s">
+      <c r="D31" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="31.2">
+      <c r="A32" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="31.5">
-      <c r="A32" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
@@ -2318,15 +2332,15 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
@@ -2334,349 +2348,349 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" ht="31.5">
+    <row r="40" spans="1:4" ht="31.2">
       <c r="A40" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="46.8">
+      <c r="A42" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="47.25">
-      <c r="A42" s="6" t="s">
+      <c r="D42" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="46.8">
+      <c r="A43" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="47.25">
-      <c r="A43" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="31.2">
+      <c r="A45" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="31.5">
-      <c r="A45" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="110.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="109.2">
       <c r="A49" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" s="13"/>
       <c r="C49" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B50" s="13"/>
       <c r="C50" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="31.5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="31.2">
       <c r="A51" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B51" s="13"/>
       <c r="C51" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="31.5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="31.2">
       <c r="A52" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B52" s="13"/>
       <c r="C52" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="31.5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="31.2">
       <c r="A53" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B55" s="13"/>
       <c r="C55" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B58" s="13"/>
       <c r="C58" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B59" s="13"/>
       <c r="C59" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="31.5">
+    <row r="61" spans="1:4" ht="31.2">
       <c r="A61" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="31.2">
+      <c r="A62" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="31.5">
-      <c r="A62" s="2" t="s">
+    </row>
+    <row r="63" spans="1:4" ht="31.2">
+      <c r="A63" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="31.5">
-      <c r="A63" s="2" t="s">
+      <c r="D63" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="31.2">
+      <c r="A64" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="31.2">
+      <c r="A65" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="31.5">
-      <c r="A64" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="31.5">
-      <c r="A65" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D65" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" ht="31.5">
+    <row r="69" spans="1:4" ht="31.2">
       <c r="A69" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:4">

</xml_diff>